<commit_message>
P07/JADE_Scrum_Sprint_2.xlsx: Updated scrum sheet
</commit_message>
<xml_diff>
--- a/P07/JADE_Scrum_Sprint_2.xlsx
+++ b/P07/JADE_Scrum_Sprint_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WASEE\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WASEE\Google Drive\Code\UVM\cse1325\P07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CF84C9-3429-40BE-A7BD-81E7AB0833B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7144097B-884B-4470-A811-211A693DD0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="204">
   <si>
     <t>Product Name:</t>
   </si>
@@ -564,13 +564,94 @@
     <t>Completed Day 6</t>
   </si>
   <si>
-    <t>"Create the store class", "Create storeName and products attributes", "Create storeName method that returns name of store", "create adddProduct method that adds a new product to products ArrayList", "create numberOfProducts method that returns the number of items in products ArrayList", "create toString method that prints a single product's information", "override toString method of the class to print all the items in the store"</t>
+    <t>Finished in Sprint 2</t>
   </si>
   <si>
-    <t>"Create a Donut class", "create the frosting, and filling enums", "create filling, frosting, and sprinkles attributes", "override toString method to print the donut name and customizations"</t>
+    <t>Create a Java (coffee) class</t>
   </si>
   <si>
-    <t>"Create a Java (coffee) class", "create the darkness and shots enums", "create darkness and shots attributes",  "create aeddShot method that adds a shot to the shots ArrayList", "override toString method to print the donut name and customizations"</t>
+    <t>create the darkness and shots enums</t>
+  </si>
+  <si>
+    <t>create darkness and shots attributes</t>
+  </si>
+  <si>
+    <t>create aeddShot method that adds a shot to the shots ArrayList</t>
+  </si>
+  <si>
+    <t>override toString method to print the donut name and customizations</t>
+  </si>
+  <si>
+    <t>Create a Donut class</t>
+  </si>
+  <si>
+    <t>create the frosting, and filling enums</t>
+  </si>
+  <si>
+    <t>create filling, frosting, and sprinkles attributes</t>
+  </si>
+  <si>
+    <t>Create the store class</t>
+  </si>
+  <si>
+    <t>of items in products ArrayList</t>
+  </si>
+  <si>
+    <t>create toString method that prints a single product's information</t>
+  </si>
+  <si>
+    <t>override toString method of the class to print all the items in the store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reorganizing Files into packages </t>
+  </si>
+  <si>
+    <t>Completed Day 2</t>
+  </si>
+  <si>
+    <t>Creating MainWin class</t>
+  </si>
+  <si>
+    <t>Completed Day 3</t>
+  </si>
+  <si>
+    <t>Creating menus and menu items to the menu bar</t>
+  </si>
+  <si>
+    <t>Creating action listeners and methods for the menu items</t>
+  </si>
+  <si>
+    <t>Creating button art</t>
+  </si>
+  <si>
+    <t>Creating buttons and their action listeners</t>
+  </si>
+  <si>
+    <t>Completed Day 4</t>
+  </si>
+  <si>
+    <t>Creating a menubar object</t>
+  </si>
+  <si>
+    <t>The class responsible for the main window of the program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creating Button pictures using Aseprite pixel art program </t>
+  </si>
+  <si>
+    <t>Creating input dialogs for  Java and Donut name, price, and cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create input dialogs with combo boxed for donut and java customizations </t>
+  </si>
+  <si>
+    <t>to select Filling, Frosting, Darkness</t>
+  </si>
+  <si>
+    <t>Create input dialogs with checkboxes for java shots</t>
+  </si>
+  <si>
+    <t>Display all products in the store to the screen</t>
   </si>
 </sst>
 </file>
@@ -1061,19 +1142,19 @@
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1357,22 +1438,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1670,28 +1751,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3728,8 +3809,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ79"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -3947,11 +4028,11 @@
       </c>
       <c r="B14" s="2">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="7">
         <f>COUNTIF(F$24:F$66,"Finished in Sprint 2")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="9">
@@ -3970,7 +4051,7 @@
       </c>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="7">
         <f>COUNTIF(F$24:F$66,"Finished in Sprint 3")</f>
@@ -3993,7 +4074,7 @@
       </c>
       <c r="B16" s="2">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="7">
         <f>COUNTIF(F$24:F$66,"Finished in Sprint 4")</f>
@@ -4012,7 +4093,7 @@
       </c>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="7">
         <f>COUNTIF(F$24:F$66,"Finished in Sprint 5")</f>
@@ -4031,7 +4112,7 @@
       </c>
       <c r="B18" s="2">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="7">
         <f>COUNTIF(F$24:F$66,"Finished in Sprint 6")</f>
@@ -4235,7 +4316,9 @@
       <c r="E27" s="15">
         <v>2</v>
       </c>
-      <c r="F27" s="15"/>
+      <c r="F27" s="15" t="s">
+        <v>174</v>
+      </c>
       <c r="G27" s="19" t="s">
         <v>31</v>
       </c>
@@ -12341,8 +12424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -12445,7 +12528,7 @@
       </c>
       <c r="B7" s="34">
         <f>COUNTA(D17:D995)</f>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
@@ -12460,7 +12543,7 @@
       </c>
       <c r="B8" s="34">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C8" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -12478,7 +12561,7 @@
       </c>
       <c r="B9" s="34">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C9" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -12496,7 +12579,7 @@
       </c>
       <c r="B10" s="34">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C10" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -12514,7 +12597,7 @@
       </c>
       <c r="B11" s="34">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C11" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -12532,11 +12615,11 @@
       </c>
       <c r="B12" s="34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C12" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
@@ -12554,7 +12637,7 @@
       </c>
       <c r="C13" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
@@ -13639,7 +13722,7 @@
         <v>170</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E17" s="39" t="s">
         <v>172</v>
@@ -13650,16 +13733,16 @@
         <v>2</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C18" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -13667,13 +13750,13 @@
         <v>3</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C19" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E19" s="39" t="s">
         <v>172</v>
@@ -13683,91 +13766,171 @@
       <c r="A20" s="37">
         <v>4</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="39"/>
+      <c r="B20" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="37">
         <v>5</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="39"/>
+      <c r="B21" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="37">
         <v>6</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="39"/>
+      <c r="B22" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="37">
         <v>7</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="39"/>
+      <c r="B23" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="37">
         <v>8</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="39"/>
+      <c r="B24" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="E24" s="39" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="37">
         <v>9</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="39"/>
+      <c r="B25" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="E25" s="39" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="37">
         <v>10</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="39"/>
+      <c r="B26" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="E26" s="39" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="37">
         <v>11</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="39"/>
+      <c r="B27" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="E27" s="39" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="37">
         <v>12</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="39"/>
+      <c r="B28" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="E28" s="39" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="37">
         <v>13</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="39"/>
+      <c r="B29" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="E29" s="39" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="37">
@@ -14414,16 +14577,16 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank until task is begun._x000a_Select &quot;In Work&quot; when started (for long tasks only)._x000a_Select Completed ONLY when this task is done._x000a_    Select &quot;Completed Day 1&quot; if finished on the first day, and_x000a_    similarly for &quot;Completed on Day 2&quot; et. al." sqref="E17:E100" xr:uid="{00000000-0002-0000-0100-000003000000}">
-      <formula1>"In Work,Completed Day 1,Completed Day 2,Completed Day 3,Completed Day 4,Completed Day 5,Completed Day 6,Completed Day 7,"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D18:D100" xr:uid="{00000000-0002-0000-0100-000005000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D18:D22 D26:D29 D31:D100" xr:uid="{00000000-0002-0000-0100-000005000000}">
       <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank until task is begun._x000a_Select &quot;In Work&quot; when started (for long tasks only)._x000a_Select Completed ONLY when this task is done._x000a_    Select &quot;Completed Day 1&quot; if finished on the first day, and_x000a_    similarly for &quot;Completed on Day 2&quot; et. al." sqref="E17:E29 E31:E100" xr:uid="{00000000-0002-0000-0100-000003000000}">
+      <formula1>"In Work,Completed Day 1,Completed Day 2,Completed Day 3,Completed Day 4,Completed Day 5,Completed Day 6,Completed Day 7,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -14444,7 +14607,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B17:B100</xm:sqref>
+          <xm:sqref>B17:B29 B31:B100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="Exactly ONE team member may be responsible for any task, and they will receive grade credit for their work._x000a__x000a_If you have more than one person on your team, each member MUST select their initials for each task the agree to perform. Use this to ensure that " xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
@@ -14453,7 +14616,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>C17:C100</xm:sqref>
+          <xm:sqref>C17:C29 C31:C100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -14465,8 +14628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -14571,7 +14734,7 @@
       </c>
       <c r="B7" s="34">
         <f>COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
@@ -14586,7 +14749,7 @@
       </c>
       <c r="B8" s="34">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C8" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -14604,11 +14767,11 @@
       </c>
       <c r="B9" s="34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C9" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
@@ -14622,11 +14785,11 @@
       </c>
       <c r="B10" s="34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C10" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
@@ -14640,11 +14803,11 @@
       </c>
       <c r="B11" s="34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
@@ -14658,7 +14821,7 @@
       </c>
       <c r="B12" s="34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -14676,7 +14839,7 @@
       </c>
       <c r="B13" s="34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -14694,7 +14857,7 @@
       </c>
       <c r="B14" s="34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -15754,108 +15917,197 @@
       <c r="AMI16" s="37"/>
       <c r="AMJ16" s="37"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" s="37">
         <v>1</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="38" t="s">
-        <v>167</v>
-      </c>
-      <c r="E17" s="39"/>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="B17" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="37">
         <v>2</v>
       </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="39"/>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="B18" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="F18" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="37">
         <v>3</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="39"/>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="B19" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="37">
         <v>4</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="39"/>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="B20" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>191</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="37">
         <v>5</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="39"/>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="B21" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="37">
         <v>6</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="39"/>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="B22" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="F22" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="37">
         <v>7</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="39"/>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="B23" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="37">
         <v>8</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="39"/>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="B24" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>199</v>
+      </c>
+      <c r="E24" s="39" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="37">
         <v>9</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="36"/>
+      <c r="B25" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>200</v>
+      </c>
       <c r="E25" s="39"/>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="37">
         <v>10</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="36"/>
+      <c r="B26" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>202</v>
+      </c>
       <c r="E26" s="39"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" s="37">
         <v>11</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="36"/>
+      <c r="B27" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>203</v>
+      </c>
       <c r="E27" s="39"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6">
       <c r="A28" s="37">
         <v>12</v>
       </c>
@@ -15864,7 +16116,7 @@
       <c r="D28" s="36"/>
       <c r="E28" s="39"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" s="37">
         <v>13</v>
       </c>
@@ -15873,7 +16125,7 @@
       <c r="D29" s="36"/>
       <c r="E29" s="39"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30" s="37">
         <v>14</v>
       </c>
@@ -15882,7 +16134,7 @@
       <c r="D30" s="36"/>
       <c r="E30" s="39"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6">
       <c r="A31" s="37">
         <v>15</v>
       </c>
@@ -15891,7 +16143,7 @@
       <c r="D31" s="36"/>
       <c r="E31" s="39"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:6">
       <c r="A32" s="37">
         <v>16</v>
       </c>
@@ -16526,7 +16778,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D18:D100" xr:uid="{00000000-0002-0000-0200-000005000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D17:D100" xr:uid="{00000000-0002-0000-0200-000005000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
P07/JADE_Scrum_Sprint_2.xlsx: Updating Sprint 2 backlog
</commit_message>
<xml_diff>
--- a/P07/JADE_Scrum_Sprint_2.xlsx
+++ b/P07/JADE_Scrum_Sprint_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WASEE\Google Drive\Code\UVM\cse1325\P07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7144097B-884B-4470-A811-211A693DD0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099E8532-7A27-498B-9956-6F6DFD3BE344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="207">
   <si>
     <t>Product Name:</t>
   </si>
@@ -652,6 +652,15 @@
   </si>
   <si>
     <t>Display all products in the store to the screen</t>
+  </si>
+  <si>
+    <t>Create a confirm dialog to ask if the donut has sprinkles or not</t>
+  </si>
+  <si>
+    <t>Only display this option if the donut has frosting</t>
+  </si>
+  <si>
+    <t>In Work</t>
   </si>
 </sst>
 </file>
@@ -1751,28 +1760,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12425,7 +12434,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -14629,7 +14638,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -14734,7 +14743,7 @@
       </c>
       <c r="B7" s="34">
         <f>COUNTA(D17:D995)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
@@ -14749,7 +14758,7 @@
       </c>
       <c r="B8" s="34">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -14767,7 +14776,7 @@
       </c>
       <c r="B9" s="34">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -14785,7 +14794,7 @@
       </c>
       <c r="B10" s="34">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -14803,7 +14812,7 @@
       </c>
       <c r="B11" s="34">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -14821,11 +14830,11 @@
       </c>
       <c r="B12" s="34">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
@@ -14839,7 +14848,7 @@
       </c>
       <c r="B13" s="34">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -14857,7 +14866,7 @@
       </c>
       <c r="B14" s="34">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -16072,7 +16081,9 @@
       <c r="D25" s="36" t="s">
         <v>200</v>
       </c>
-      <c r="E25" s="39"/>
+      <c r="E25" s="39" t="s">
+        <v>172</v>
+      </c>
       <c r="F25" t="s">
         <v>201</v>
       </c>
@@ -16090,7 +16101,9 @@
       <c r="D26" s="36" t="s">
         <v>202</v>
       </c>
-      <c r="E26" s="39"/>
+      <c r="E26" s="39" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="37">
@@ -16111,10 +16124,21 @@
       <c r="A28" s="37">
         <v>12</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="39"/>
+      <c r="B28" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" s="36" t="s">
+        <v>204</v>
+      </c>
+      <c r="E28" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="F28" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="37">

</xml_diff>

<commit_message>
P07/JADE_Scrum_Sprint_2.xlsx: Updated sprint 2 backlog
</commit_message>
<xml_diff>
--- a/P07/JADE_Scrum_Sprint_2.xlsx
+++ b/P07/JADE_Scrum_Sprint_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WASEE\Google Drive\Code\UVM\cse1325\P07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099E8532-7A27-498B-9956-6F6DFD3BE344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D7CF1C-1C93-4262-84D8-570BD34F7B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="206">
   <si>
     <t>Product Name:</t>
   </si>
@@ -648,9 +648,6 @@
     <t>to select Filling, Frosting, Darkness</t>
   </si>
   <si>
-    <t>Create input dialogs with checkboxes for java shots</t>
-  </si>
-  <si>
     <t>Display all products in the store to the screen</t>
   </si>
   <si>
@@ -660,7 +657,7 @@
     <t>Only display this option if the donut has frosting</t>
   </si>
   <si>
-    <t>In Work</t>
+    <t>Create an about dialog with the logo, prgram version and copyright, along with  appropriate creditation</t>
   </si>
 </sst>
 </file>
@@ -672,7 +669,7 @@
     <numFmt numFmtId="165" formatCode="mmm\ dd"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -742,6 +739,11 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1151,19 +1153,19 @@
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1778,10 +1780,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3818,8 +3820,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ79"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K29" sqref="K28:K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -4037,11 +4039,11 @@
       </c>
       <c r="B14" s="2">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="7">
         <f>COUNTIF(F$24:F$66,"Finished in Sprint 2")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="9">
@@ -4060,7 +4062,7 @@
       </c>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="7">
         <f>COUNTIF(F$24:F$66,"Finished in Sprint 3")</f>
@@ -4083,7 +4085,7 @@
       </c>
       <c r="B16" s="2">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="7">
         <f>COUNTIF(F$24:F$66,"Finished in Sprint 4")</f>
@@ -4102,7 +4104,7 @@
       </c>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="7">
         <f>COUNTIF(F$24:F$66,"Finished in Sprint 5")</f>
@@ -4121,7 +4123,7 @@
       </c>
       <c r="B18" s="2">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="7">
         <f>COUNTIF(F$24:F$66,"Finished in Sprint 6")</f>
@@ -4357,7 +4359,9 @@
       <c r="E28" s="15">
         <v>2</v>
       </c>
-      <c r="F28" s="15"/>
+      <c r="F28" s="15" t="s">
+        <v>174</v>
+      </c>
       <c r="G28" s="19" t="s">
         <v>31</v>
       </c>
@@ -4384,7 +4388,9 @@
       <c r="D29" s="25">
         <v>13</v>
       </c>
-      <c r="E29" s="15"/>
+      <c r="E29" s="15">
+        <v>3</v>
+      </c>
       <c r="F29" s="15"/>
       <c r="G29" s="16" t="s">
         <v>31</v>
@@ -4412,7 +4418,9 @@
       <c r="D30" s="25">
         <v>8</v>
       </c>
-      <c r="E30" s="15"/>
+      <c r="E30" s="15">
+        <v>3</v>
+      </c>
       <c r="F30" s="15"/>
       <c r="G30" s="16" t="s">
         <v>31</v>
@@ -4440,7 +4448,9 @@
       <c r="D31" s="25">
         <v>5</v>
       </c>
-      <c r="E31" s="15"/>
+      <c r="E31" s="15">
+        <v>3</v>
+      </c>
       <c r="F31" s="15"/>
       <c r="G31" s="16" t="s">
         <v>31</v>
@@ -4468,7 +4478,9 @@
       <c r="D32" s="25">
         <v>5</v>
       </c>
-      <c r="E32" s="15"/>
+      <c r="E32" s="15">
+        <v>3</v>
+      </c>
       <c r="F32" s="15"/>
       <c r="G32" s="16" t="s">
         <v>57</v>
@@ -4496,7 +4508,9 @@
       <c r="D33" s="25">
         <v>5</v>
       </c>
-      <c r="E33" s="15"/>
+      <c r="E33" s="15">
+        <v>3</v>
+      </c>
       <c r="F33" s="15"/>
       <c r="G33" s="16" t="s">
         <v>57</v>
@@ -5538,7 +5552,9 @@
       <c r="D34" s="18">
         <v>5</v>
       </c>
-      <c r="E34" s="15"/>
+      <c r="E34" s="15">
+        <v>4</v>
+      </c>
       <c r="F34" s="15"/>
       <c r="G34" s="19" t="s">
         <v>64</v>
@@ -6580,7 +6596,9 @@
       <c r="D35" s="18">
         <v>2</v>
       </c>
-      <c r="E35" s="15"/>
+      <c r="E35" s="15">
+        <v>4</v>
+      </c>
       <c r="F35" s="15"/>
       <c r="G35" s="19" t="s">
         <v>69</v>
@@ -6606,7 +6624,9 @@
       <c r="D36" s="18">
         <v>8</v>
       </c>
-      <c r="E36" s="15"/>
+      <c r="E36" s="15">
+        <v>4</v>
+      </c>
       <c r="F36" s="15"/>
       <c r="G36" s="19" t="s">
         <v>69</v>
@@ -6632,7 +6652,9 @@
       <c r="D37" s="18">
         <v>3</v>
       </c>
-      <c r="E37" s="15"/>
+      <c r="E37" s="15">
+        <v>4</v>
+      </c>
       <c r="F37" s="15"/>
       <c r="G37" s="19" t="s">
         <v>64</v>
@@ -6660,7 +6682,9 @@
       <c r="D38" s="18">
         <v>8</v>
       </c>
-      <c r="E38" s="15"/>
+      <c r="E38" s="15">
+        <v>4</v>
+      </c>
       <c r="F38" s="15"/>
       <c r="G38" s="19" t="s">
         <v>64</v>
@@ -6688,7 +6712,9 @@
       <c r="D39" s="25">
         <v>5</v>
       </c>
-      <c r="E39" s="15"/>
+      <c r="E39" s="15">
+        <v>5</v>
+      </c>
       <c r="F39" s="15"/>
       <c r="G39" s="16" t="s">
         <v>69</v>
@@ -6714,7 +6740,9 @@
       <c r="D40" s="25">
         <v>3</v>
       </c>
-      <c r="E40" s="15"/>
+      <c r="E40" s="15">
+        <v>5</v>
+      </c>
       <c r="F40" s="15"/>
       <c r="G40" s="16" t="s">
         <v>57</v>
@@ -6740,7 +6768,9 @@
       <c r="D41" s="25">
         <v>8</v>
       </c>
-      <c r="E41" s="15"/>
+      <c r="E41" s="15">
+        <v>5</v>
+      </c>
       <c r="F41" s="15"/>
       <c r="G41" s="16" t="s">
         <v>31</v>
@@ -6768,7 +6798,9 @@
       <c r="D42" s="25">
         <v>8</v>
       </c>
-      <c r="E42" s="15"/>
+      <c r="E42" s="15">
+        <v>5</v>
+      </c>
       <c r="F42" s="15"/>
       <c r="G42" s="16" t="s">
         <v>31</v>
@@ -7810,7 +7842,9 @@
       <c r="D43" s="18">
         <v>21</v>
       </c>
-      <c r="E43" s="15"/>
+      <c r="E43" s="15">
+        <v>6</v>
+      </c>
       <c r="F43" s="15"/>
       <c r="G43" s="19" t="s">
         <v>31</v>
@@ -8852,7 +8886,9 @@
       <c r="D44" s="18">
         <v>8</v>
       </c>
-      <c r="E44" s="15"/>
+      <c r="E44" s="15">
+        <v>6</v>
+      </c>
       <c r="F44" s="15"/>
       <c r="G44" s="19" t="s">
         <v>31</v>
@@ -12410,7 +12446,7 @@
       <formula1>"0,1,2,3,5,8,13,21,34,55,89"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Sprint" prompt="Select the sprint number (1, 2, etc.) in which you plan to implement this feature.  This is just for planning purposes, it won't affect your grade._x000a__x000a_In Scrum, you only plan the current sprint, not future sprints, so you don't need to fill this in for any " sqref="E24:E44 E48:E61" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Sprint" prompt="Select the sprint number (1, 2, etc.) in which you plan to implement this feature.  This is just for planning purposes, it won't affect your grade._x000a__x000a_In Scrum, you only plan the current sprint, not future sprints, so you don't need to fill this in for any " sqref="E48:E61 E24:E44" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"1,2,3,4,5,6"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -14637,8 +14673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -14848,11 +14884,11 @@
       </c>
       <c r="B13" s="34">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C13" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
@@ -14866,7 +14902,7 @@
       </c>
       <c r="B14" s="34">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C14" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -16093,7 +16129,7 @@
         <v>10</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C26" s="37" t="s">
         <v>170</v>
@@ -16102,7 +16138,7 @@
         <v>202</v>
       </c>
       <c r="E26" s="39" t="s">
-        <v>206</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -16110,7 +16146,7 @@
         <v>11</v>
       </c>
       <c r="B27" s="36" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C27" s="37" t="s">
         <v>170</v>
@@ -16118,7 +16154,12 @@
       <c r="D27" s="36" t="s">
         <v>203</v>
       </c>
-      <c r="E27" s="39"/>
+      <c r="E27" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="F27" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="37">
@@ -16131,13 +16172,10 @@
         <v>170</v>
       </c>
       <c r="D28" s="36" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E28" s="39" t="s">
-        <v>172</v>
-      </c>
-      <c r="F28" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -16789,6 +16827,7 @@
       <c r="E100" s="39"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="4">
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task ID" prompt="This is just an arbitrary unique (per sprint) integer assigned to a task, used by the team to refer to that task. " sqref="A17:A100" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>0</formula1>
@@ -16798,11 +16837,11 @@
       <formula1>"In Work,Completed Day 1,Completed Day 2,Completed Day 3,Completed Day 4,Completed Day 5,Completed Day 6,Completed Day 7,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100" xr:uid="{00000000-0002-0000-0200-000004000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D29:D100 D17:D27" xr:uid="{00000000-0002-0000-0200-000005000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D17:D100" xr:uid="{00000000-0002-0000-0200-000005000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F29:F100 F17:F27" xr:uid="{00000000-0002-0000-0200-000004000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -16824,7 +16863,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B17:B100</xm:sqref>
+          <xm:sqref>B29:B100 B17:B27</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="Exactly ONE team member may be responsible for any task, and they will receive grade credit for their work._x000a__x000a_If you have more than one person on your team, each member MUST select their initials for each task the agree to perform. Use this to ensure that " xr:uid="{00000000-0002-0000-0200-000002000000}">
           <x14:formula1>
@@ -16833,7 +16872,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>C17:C100</xm:sqref>
+          <xm:sqref>C29:C100 C17:C27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>